<commit_message>
Adding 2D plotting script with gif!
</commit_message>
<xml_diff>
--- a/scenarios/scenario1_results/results_tabulated.xlsx
+++ b/scenarios/scenario1_results/results_tabulated.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Agility" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="10">
   <si>
     <t xml:space="preserve">Config</t>
   </si>
@@ -42,6 +42,9 @@
   </si>
   <si>
     <t xml:space="preserve">All with 50% flooded</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All with 10% flooded</t>
   </si>
   <si>
     <t xml:space="preserve">Unique alt outliers</t>
@@ -160,15 +163,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.35"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -259,6 +262,97 @@
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" s="1" t="n">
+        <v>4E-007</v>
+      </c>
+      <c r="C9" s="1" t="n">
+        <v>4E-005</v>
+      </c>
+      <c r="D9" s="1" t="n">
+        <v>0.004</v>
+      </c>
+      <c r="E9" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="D10" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="E10" s="0" t="n">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <v>36</v>
+      </c>
+      <c r="D11" s="0" t="n">
+        <v>41</v>
+      </c>
+      <c r="E11" s="0" t="n">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" s="0" t="n">
+        <v>48</v>
+      </c>
+      <c r="C12" s="0" t="n">
+        <v>58</v>
+      </c>
+      <c r="D12" s="0" t="n">
+        <v>58</v>
+      </c>
+      <c r="E12" s="0" t="n">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" s="0" t="n">
+        <v>38</v>
+      </c>
+      <c r="C13" s="0" t="n">
+        <v>37</v>
+      </c>
+      <c r="D13" s="0" t="n">
+        <v>39</v>
+      </c>
+      <c r="E13" s="0" t="n">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -279,11 +373,11 @@
   </sheetPr>
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C34" activeCellId="0" sqref="C34"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -301,7 +395,7 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B2" s="3" t="n">
         <v>508</v>
@@ -371,7 +465,7 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>